<commit_message>
Atualização automática de GUARANI_DAS_MISSOES.xlsx
</commit_message>
<xml_diff>
--- a/GUARANI_DAS_MISSOES.xlsx
+++ b/GUARANI_DAS_MISSOES.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gera-fichas\Comarcas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{13FE9B9C-C33C-4EDD-BE6A-DB87F7C7AF58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6EAC67C1-024A-480A-AA3D-AAD48B7198BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1042,7 +1042,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -1102,36 +1102,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1170,14 +1146,9 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1207,7 +1178,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="1" xr:uid="{C01E7794-24AD-42B3-92C1-1C7CE13D3DE5}"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{A7A37823-E3DC-4DAA-865F-4C14DD35AEA9}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1237,10 +1208,10 @@
         <xdr:cNvPr id="2" name="Chart1" title="Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{28C59BF2-D7E3-40EC-AD25-2967BA295BCD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DC5E98CF-69FC-4EB3-B1D0-79A7651C447D}"/>
             </a:ext>
             <a:ext uri="GoogleSheetsCustomDataVersion1">
-              <go:sheetsCustomData xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:go="http://customooxmlschemas.google.com/" pictureOfChart="1"/>
+              <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" pictureOfChart="1"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1278,7 +1249,7 @@
         <xdr:cNvPr id="3" name="Shape 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C20096D7-C7C1-452E-806B-1B65CCA29566}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3D802E7B-E696-4CBB-AE4B-536FFB260492}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1341,7 +1312,7 @@
         <xdr:cNvPr id="4" name="Shape 2" title="Desenho">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{457B94A9-F2C4-4F5A-9A05-71A228612478}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{095DFD7A-DC75-401F-8D3B-69B0BBAFE8DA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1360,7 +1331,7 @@
           <xdr:cNvPr id="5" name="Shape 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{937A3C38-ED29-DFA0-6B9D-2666ADCA32AF}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6E2DF42B-B456-C32E-0FA1-A486521CF9FC}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1409,7 +1380,7 @@
           <xdr:cNvPr id="6" name="Shape 5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FDF5694E-AA3E-02A2-12F2-A009C5A59381}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{059C867F-FD17-C6C8-F849-0AD76B00E817}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1428,7 +1399,7 @@
             <xdr:cNvPr id="7" name="Shape 6">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{022C4CFD-C23D-0909-FE37-2D56066C0706}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D414D223-D267-952E-B39E-3E1EF49B2961}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1459,7 +1430,7 @@
             <xdr:cNvPr id="8" name="Shape 7">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{90AA77AC-7F1C-A6CD-4D47-EF7137FF5D8A}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F2725BD7-F15F-0B01-BEDE-6F41506B341E}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1490,7 +1461,7 @@
             <xdr:cNvPr id="9" name="Shape 8">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3491D17F-32D0-4D03-FE7A-7C6D87056797}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3F124FE7-7778-4870-8C36-3D0F0CADECA6}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1533,7 +1504,7 @@
         <xdr:cNvPr id="10" name="image2.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{46120C58-2635-4E46-ADB4-F5EA2EC72AC7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{75755B77-748E-4E50-9AD3-18AD89790194}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1571,7 +1542,7 @@
         <xdr:cNvPr id="11" name="image1.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DB8B2B2D-AFCD-489D-9188-FC43F76D622C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E3838852-88FF-4700-A9FA-FAF75D626651}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1614,7 +1585,7 @@
         <xdr:cNvPr id="12" name="Imagem 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7CC6A933-C3A1-4433-9F25-D39612952205}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E29D1627-D173-4FD0-92FB-5DCC9DD659E9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1927,7 +1898,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{153A8504-FA9E-4391-9D00-CC81786B40C3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40C16638-A708-4BE3-8BED-C8CC52B2AAF7}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -1939,98 +1910,98 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="5" width="12.5703125" style="31"/>
-    <col min="6" max="6" width="2" style="31" customWidth="1"/>
-    <col min="7" max="16" width="13.42578125" style="31" customWidth="1"/>
-    <col min="17" max="16384" width="12.5703125" style="31"/>
+    <col min="1" max="5" width="12.5703125" style="28"/>
+    <col min="6" max="6" width="2" style="28" customWidth="1"/>
+    <col min="7" max="16" width="13.42578125" style="28" customWidth="1"/>
+    <col min="17" max="16384" width="12.5703125" style="28"/>
   </cols>
   <sheetData>
     <row r="1" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F1" s="30"/>
+      <c r="F1" s="27"/>
     </row>
     <row r="2" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F2" s="30"/>
+      <c r="F2" s="27"/>
     </row>
     <row r="3" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F3" s="30"/>
+      <c r="F3" s="27"/>
     </row>
     <row r="4" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F4" s="30"/>
+      <c r="F4" s="27"/>
     </row>
     <row r="5" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F5" s="30"/>
+      <c r="F5" s="27"/>
     </row>
     <row r="6" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F6" s="30"/>
+      <c r="F6" s="27"/>
     </row>
     <row r="7" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F7" s="30"/>
+      <c r="F7" s="27"/>
     </row>
     <row r="8" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F8" s="30"/>
+      <c r="F8" s="27"/>
     </row>
     <row r="9" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F9" s="30"/>
+      <c r="F9" s="27"/>
     </row>
     <row r="10" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F10" s="30"/>
+      <c r="F10" s="27"/>
     </row>
     <row r="11" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F11" s="30"/>
+      <c r="F11" s="27"/>
     </row>
     <row r="12" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F12" s="30"/>
+      <c r="F12" s="27"/>
     </row>
     <row r="13" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F13" s="30"/>
+      <c r="F13" s="27"/>
     </row>
     <row r="14" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F14" s="30"/>
+      <c r="F14" s="27"/>
     </row>
     <row r="15" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F15" s="30"/>
+      <c r="F15" s="27"/>
     </row>
     <row r="16" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F16" s="30"/>
+      <c r="F16" s="27"/>
     </row>
     <row r="17" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F17" s="30"/>
+      <c r="F17" s="27"/>
     </row>
     <row r="18" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F18" s="30"/>
+      <c r="F18" s="27"/>
     </row>
     <row r="19" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F19" s="30"/>
+      <c r="F19" s="27"/>
     </row>
     <row r="20" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F20" s="30"/>
+      <c r="F20" s="27"/>
     </row>
     <row r="21" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F21" s="30"/>
+      <c r="F21" s="27"/>
     </row>
     <row r="22" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F22" s="30"/>
+      <c r="F22" s="27"/>
     </row>
     <row r="23" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F23" s="30"/>
+      <c r="F23" s="27"/>
     </row>
     <row r="24" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F24" s="30"/>
+      <c r="F24" s="27"/>
     </row>
     <row r="25" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F25" s="30"/>
+      <c r="F25" s="27"/>
     </row>
     <row r="26" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F26" s="30"/>
+      <c r="F26" s="27"/>
     </row>
     <row r="27" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F27" s="30"/>
+      <c r="F27" s="27"/>
     </row>
     <row r="28" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F28" s="30"/>
+      <c r="F28" s="27"/>
     </row>
     <row r="29" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F29" s="30"/>
+      <c r="F29" s="27"/>
     </row>
   </sheetData>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -5260,19 +5231,19 @@
     <col min="2" max="2" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="16" t="s">
         <v>269</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="2" t="s">
         <v>270</v>
       </c>
     </row>
@@ -5295,46 +5266,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="18" t="s">
         <v>271</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="17" t="s">
         <v>272</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="19" t="s">
         <v>273</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="C2" s="19" t="s">
         <v>274</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="19" t="s">
         <v>275</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="19" t="s">
         <v>274</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="19" t="s">
         <v>276</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="19" t="s">
         <v>274</v>
       </c>
     </row>
@@ -5359,54 +5330,55 @@
     <col min="6" max="6" width="12.5703125" customWidth="1"/>
     <col min="7" max="7" width="13" customWidth="1"/>
     <col min="8" max="8" width="15.42578125" customWidth="1"/>
-    <col min="9" max="14" width="13" customWidth="1"/>
-    <col min="15" max="15" width="30.85546875" customWidth="1"/>
+    <col min="9" max="12" width="13" customWidth="1"/>
+    <col min="13" max="13" width="42.140625" customWidth="1"/>
+    <col min="14" max="15" width="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="20" t="s">
         <v>277</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="21" t="s">
         <v>278</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="21" t="s">
         <v>279</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="21" t="s">
         <v>280</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="E1" s="21" t="s">
         <v>281</v>
       </c>
-      <c r="F1" s="25" t="s">
+      <c r="F1" s="22" t="s">
         <v>282</v>
       </c>
-      <c r="G1" s="25" t="s">
+      <c r="G1" s="22" t="s">
         <v>283</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="20" t="s">
         <v>284</v>
       </c>
-      <c r="I1" s="23" t="s">
+      <c r="I1" s="20" t="s">
         <v>285</v>
       </c>
-      <c r="J1" s="23" t="s">
+      <c r="J1" s="20" t="s">
         <v>286</v>
       </c>
-      <c r="K1" s="23" t="s">
+      <c r="K1" s="20" t="s">
         <v>287</v>
       </c>
-      <c r="L1" s="23" t="s">
+      <c r="L1" s="20" t="s">
         <v>288</v>
       </c>
-      <c r="M1" s="23" t="s">
+      <c r="M1" s="20" t="s">
         <v>289</v>
       </c>
-      <c r="N1" s="23" t="s">
+      <c r="N1" s="20" t="s">
         <v>290</v>
       </c>
-      <c r="O1" s="23" t="s">
+      <c r="O1" s="20" t="s">
         <v>291</v>
       </c>
     </row>
@@ -5417,41 +5389,41 @@
       <c r="B2" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="C2" s="26">
+      <c r="C2" s="23">
         <v>45901</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="F2" s="27">
+      <c r="F2" s="24">
         <v>0</v>
       </c>
-      <c r="G2" s="27">
+      <c r="G2" s="24">
         <v>0</v>
       </c>
-      <c r="H2" s="28" t="s">
+      <c r="H2" s="25" t="s">
         <v>294</v>
       </c>
-      <c r="I2" s="28" t="s">
+      <c r="I2" s="25" t="s">
         <v>294</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="K2" s="28" t="s">
+      <c r="K2" s="25" t="s">
         <v>294</v>
       </c>
-      <c r="L2" s="28" t="s">
+      <c r="L2" s="25" t="s">
         <v>294</v>
       </c>
-      <c r="M2" s="28" t="s">
+      <c r="M2" s="25" t="s">
         <v>294</v>
       </c>
       <c r="N2" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="O2" s="29" t="s">
+      <c r="O2" s="26" t="s">
         <v>296</v>
       </c>
     </row>

</xml_diff>